<commit_message>
I made changes in to the print lines to make them more clear...if something doesn't work go back one commit.
</commit_message>
<xml_diff>
--- a/Stereotaxic Parts List.xlsx
+++ b/Stereotaxic Parts List.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01bcc1a4e60e225b/Active Folder/Programming/PycharmProjects/Stereotaxiccontrol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="369" documentId="8_{C5FEC8E3-01B7-4CE6-A30C-16EEB4E1FDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FA18972-4703-4DAE-970D-57E52A2C4087}"/>
+  <xr:revisionPtr revIDLastSave="433" documentId="8_{C5FEC8E3-01B7-4CE6-A30C-16EEB4E1FDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7AEC771-5B0E-4024-9C92-1D1CEE0940BB}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" activeTab="1" xr2:uid="{91600FFD-6F05-46D3-8830-DE4393442829}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" activeTab="1" xr2:uid="{91600FFD-6F05-46D3-8830-DE4393442829}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts Sheet - IC debouncer" sheetId="3" r:id="rId1"/>
     <sheet name="Parts Sheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Old sheet" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Old sheet" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="111">
   <si>
     <t>Digikey.ca</t>
   </si>
@@ -317,13 +318,68 @@
   </si>
   <si>
     <t xml:space="preserve">	B083YTPYYQ</t>
+  </si>
+  <si>
+    <t>‎B0CDBC81MG</t>
+  </si>
+  <si>
+    <t>Micro USB Male Type B 5 Terminal Jack Port Solder Connector</t>
+  </si>
+  <si>
+    <t>B079Z8RTSM</t>
+  </si>
+  <si>
+    <t>B0D1QFFHDK</t>
+  </si>
+  <si>
+    <t>1 per</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Part number</t>
+  </si>
+  <si>
+    <t>per unit price</t>
+  </si>
+  <si>
+    <t>number piece required</t>
+  </si>
+  <si>
+    <t>$12 for 20 pack</t>
+  </si>
+  <si>
+    <t>$18 for 2 pack</t>
+  </si>
+  <si>
+    <t>$11 for 10 pack</t>
+  </si>
+  <si>
+    <t>$18 for 10 pack</t>
+  </si>
+  <si>
+    <t>$16 for 5 pack</t>
+  </si>
+  <si>
+    <t>Order volume</t>
+  </si>
+  <si>
+    <t>Female Power Jack 5.5x2.5mm</t>
+  </si>
+  <si>
+    <t>Rii USB wireless keyboard (or similar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -357,15 +413,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -373,12 +441,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -395,6 +478,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1400,10 +1500,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1472,7 +1572,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G30" si="0">E3*F3</f>
+        <f t="shared" ref="G3:G29" si="0">E3*F3</f>
         <v>3.84</v>
       </c>
     </row>
@@ -1683,30 +1783,30 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="C13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="12">
         <v>17.989999999999998</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="12">
         <f t="shared" si="0"/>
         <v>17.989999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1725,41 +1825,42 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="11">
         <v>9001</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="12">
         <v>49.95</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="12">
         <f t="shared" si="0"/>
         <v>49.95</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="2">
+      <c r="D16" s="11"/>
+      <c r="E16" s="12">
         <v>35</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -1850,296 +1951,296 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
+      <c r="F21">
         <v>6</v>
       </c>
-      <c r="E21" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="2">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>6</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="12">
+        <v>60</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="12">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="15">
+        <v>19</v>
+      </c>
+      <c r="F25" s="13">
+        <v>1</v>
+      </c>
+      <c r="G25" s="15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="12">
+        <v>9</v>
+      </c>
+      <c r="F26" s="10">
         <v>2</v>
       </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="2">
-        <v>60</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="2">
-        <v>19</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="2">
-        <v>28</v>
-      </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="G27" s="2">
-        <f t="shared" si="0"/>
-        <v>56</v>
+      <c r="G26" s="12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="12">
+        <v>25</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="12">
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="E28" s="2">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E29" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E30" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" ref="G30:G31" si="1">E30*F30</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="12">
+        <v>3</v>
+      </c>
+      <c r="F31" s="10">
+        <v>1</v>
+      </c>
+      <c r="G31" s="12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="12">
+        <v>3</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1</v>
+      </c>
+      <c r="G32" s="12">
+        <f t="shared" ref="G32" si="2">E32*F32</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="12">
         <v>2</v>
       </c>
-      <c r="G30" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="2">
-        <v>10</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" s="2">
-        <f t="shared" ref="G31:G32" si="1">E31*F31</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="2">
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" s="2">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="2">
-        <v>3</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2">
-        <f t="shared" ref="G33" si="2">E33*F33</f>
-        <v>3</v>
+      <c r="F33" s="10">
+        <v>3</v>
+      </c>
+      <c r="G33" s="12">
+        <f t="shared" ref="G33:G34" si="3">E33*F33</f>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" ref="G34" si="3">E34*F34</f>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -2185,6 +2286,11 @@
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2194,6 +2300,245 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDA1B17-8C3C-4C10-A40A-336668760147}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="51.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="19">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="18">
+        <v>9001</v>
+      </c>
+      <c r="D3" s="19">
+        <v>49.95</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19">
+        <v>35</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="19">
+        <v>60</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="19">
+        <v>9</v>
+      </c>
+      <c r="E7" s="17">
+        <v>2</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="19">
+        <v>25</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="19">
+        <v>3</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="19">
+        <v>3</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="19">
+        <v>2</v>
+      </c>
+      <c r="E11" s="17">
+        <v>3</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838F9AFB-6B4A-43B0-9CD9-AA347CD8C7CB}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>